<commit_message>
added spreadshee to parse, now its good
</commit_message>
<xml_diff>
--- a/BadEventsV4ToParse.xlsx
+++ b/BadEventsV4ToParse.xlsx
@@ -26,62 +26,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="98">
   <si>
     <t>Event</t>
   </si>
   <si>
-    <t>Option 1</t>
-  </si>
-  <si>
-    <t>Option 2</t>
-  </si>
-  <si>
-    <t>Option 3</t>
-  </si>
-  <si>
-    <t>Option 4</t>
-  </si>
-  <si>
-    <t>Earthquake</t>
-  </si>
-  <si>
-    <t>Avalanche</t>
-  </si>
-  <si>
-    <t>Bad Event</t>
-  </si>
-  <si>
-    <t>Tornadoes</t>
-  </si>
-  <si>
-    <t>Exile Heretic (dream in night to priest)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You summon light rain! </t>
-  </si>
-  <si>
-    <t>Wildfires in progress</t>
-  </si>
-  <si>
-    <t>Redirect the winds (I)</t>
-  </si>
-  <si>
-    <t>Smite Heretic (I)</t>
-  </si>
-  <si>
     <t>A follower wishes to throw a fesitval in your name but is struggling to find the funds and theme.</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>The follower was only able to muster up enough to throw a small get together with friends and family. The follower tries to reconnect with his dissapointed father who wished for his son to become a tax collector. He fails.</t>
   </si>
   <si>
-    <t>The dry floor of the desert sand cracks, wells run dry, plants wilt. A drought has plagued your people.  (I)</t>
-  </si>
-  <si>
     <t>You conjure up a typhoon large enough that even you can see from your throne! As floods ravage the sparse land, your followers at lower elevations literally drown in your grace. Those few who were spared at least knew you had good intentions.</t>
   </si>
   <si>
@@ -91,93 +46,15 @@
     <t xml:space="preserve">Holiday of some sort </t>
   </si>
   <si>
-    <t>More than half empowered, win</t>
-  </si>
-  <si>
-    <t>Full empowerment, blazing victory, slaves obtained, tons of new people!</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Focus sun energy on avalanche location.</t>
-  </si>
-  <si>
-    <t>raging winds to clear the snow, saves lives of followers</t>
-  </si>
-  <si>
     <t>One "follower" has started a movement against Your Grace as he believes the "silly" array of daily rituals such as the Holy Jumping Jacks are unnecessary.</t>
   </si>
   <si>
-    <t>CANT HAPPEN: CANNOT APPEAR IN RAW PHYSICAL FORM AS GOD IN THE PHYSICAL WORLD (meaning not coming in as all powerful)</t>
-  </si>
-  <si>
-    <t>Waiting for the heretic to fall into a deep sleep, you invade his peaceful dreams and attempt to display just (???)</t>
-  </si>
-  <si>
-    <t>Your followers have gotten</t>
-  </si>
-  <si>
     <t>One follower claims to be a reincarnation of Your Grace and is speaking in your place. (?)</t>
   </si>
   <si>
     <t>You dump a good portion of your chalice on to the lands below. A thunder storm forms and rain rages down. Your followers fill their dry buckets; all are content as there is more than enough water to go around.</t>
   </si>
   <si>
-    <t>You take a heaping sip of water from your chalice and spit it out with much force. An awesome hurricane forms accompanied by biblical winds. Those with more stable housing fill their buckets without fear while (???)</t>
-  </si>
-  <si>
-    <t>A volcano dormant for thousands of years rumbles close to your people. Unknown to your people, this volcano is bound to blow soon (???)</t>
-  </si>
-  <si>
-    <t>Neighboring nation is attacking???</t>
-  </si>
-  <si>
-    <t>Oracle vision.</t>
-  </si>
-  <si>
-    <t>Punch the earth, counter earth quake</t>
-  </si>
-  <si>
-    <t>Levitate the people :D</t>
-  </si>
-  <si>
-    <t>Big robots appear from outer space, alien robots.</t>
-  </si>
-  <si>
-    <t>Pirates?</t>
-  </si>
-  <si>
-    <t>Nomad tribe</t>
-  </si>
-  <si>
-    <t>Different Severities: Mild - Do Option 1 to win, 3 - 4 is too much | Moderate - Option 1 is too little Option 4 is too much | Severe - Option 1-3 too little, option 4 good</t>
-  </si>
-  <si>
-    <t>More likely to win with power relative to option but could still lose.</t>
-  </si>
-  <si>
-    <t>Option 1 Good</t>
-  </si>
-  <si>
-    <t>Option 1 Bad</t>
-  </si>
-  <si>
-    <t>Option 2 Good</t>
-  </si>
-  <si>
-    <t>Option 2 Bad</t>
-  </si>
-  <si>
-    <t>Option 3 Good</t>
-  </si>
-  <si>
-    <t>Option 4 Bad</t>
-  </si>
-  <si>
-    <t>A neighboring nation has disrupted your peoples trade route.</t>
-  </si>
-  <si>
     <t>Water is being rationed off amongst your people, those with lower social status thirst and ask for your help.</t>
   </si>
   <si>
@@ -187,30 +64,6 @@
     <t>A volcano dormant for thousands of years rumbles close to your people. Unknown to your people, this volcano is bound to blow soon.</t>
   </si>
   <si>
-    <t>An unorganized nomad tribe has stumbled upon your peoples land and has started attacking your people.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Without much effort, you dip your fingers in your chalice and lightly sprinkle the sparse land below. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">You dump a good portion of your chalice on to the lands below. </t>
-  </si>
-  <si>
-    <t>You take a heaping sip of water from your chalice and spit it out with much force.</t>
-  </si>
-  <si>
-    <t>Option 3 Bad</t>
-  </si>
-  <si>
-    <t>Option 4 Good</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You conjure up a typhoon large enough that even you can see from your throne! </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neighboring nation has initiated an attack against your people. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Without much effort, you dip your fingers in your chalice and lightly sprinkle the sparse land below. The people are happy that rain has come their way. Some feel that this is a good sign and are gambling more </t>
   </si>
   <si>
@@ -223,12 +76,6 @@
     <t>You dump a good portion of your chalice on to the lands below. You seemed to have focused your water on one location, as a result, minor flooding occurs.</t>
   </si>
   <si>
-    <t>Event : Description of Event</t>
-  </si>
-  <si>
-    <t>Outcome is God Action : People Response</t>
-  </si>
-  <si>
     <t>You take a heaping sip of water from your chalice and spit it out with much force. People rejoice as a hurricane ravages through the lands.</t>
   </si>
   <si>
@@ -283,9 +130,6 @@
     <t>You reach to the sun and scoop a mighty fire-ball then drop it upon the rebellious movement. Many people died, but most of them were rebels… you know… probably.</t>
   </si>
   <si>
-    <t>Using your brush of magnificence, you paint the sky with a marvelous rainbow. Your people are amused.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> You take a heaping sip of water from your chalice and spit it out with much force.  A large hurricane forms over your peoples land, the winds ravage and tear up the houses of your people.</t>
   </si>
   <si>
@@ -470,24 +314,6 @@
   </si>
   <si>
     <t>There was a laughter epidemic.</t>
-  </si>
-  <si>
-    <t>As the giant robots descend, you quickly replace the ground below them with quicksand. Your followers fear quickly turns into laughter.(GOOD 5)</t>
-  </si>
-  <si>
-    <t>You summon a drizzle of rain. The robots quickly short circuit and explode.  A few unlucky followers were recipients of shrapnel to their cranial area. (BAD 5)</t>
-  </si>
-  <si>
-    <t>You open a time rift from another dimension and summon the holy tank ready for command by your people (GOOD 15).</t>
-  </si>
-  <si>
-    <t>You smite the giant robot with a bolt of lightning, with its batteries recharged it moves on its way for destruction. (BAD 15)</t>
-  </si>
-  <si>
-    <t>You snap your fingers and the robots spontenaously explode. You quietly yet confidently say "got 'em" as the accompanied wind blows shrapnel into a nearby non-worshiping nation. (GOOD 20)</t>
-  </si>
-  <si>
-    <t>You snap your fingers and the robots spontenaously explode. You quietly yet confidently say "got 'em… oh wait" as the lack of wind allows shrapnel to rain down on your folllowers. (BAD 20)</t>
   </si>
   <si>
     <t>BLANK</t>
@@ -827,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,611 +678,573 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>153</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1486,52 +1274,52 @@
     </row>
     <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -1564,125 +1352,125 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>122</v>
+        <v>70</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>141</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>142</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
another update to stuff
</commit_message>
<xml_diff>
--- a/BadEventsV4ToParse.xlsx
+++ b/BadEventsV4ToParse.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="122">
   <si>
     <t>Event</t>
   </si>
@@ -67,9 +67,6 @@
     <t xml:space="preserve">Without much effort, you dip your fingers in your chalice and lightly sprinkle the sparse land below. The people are happy that rain has come their way. Some feel that this is a good sign and are gambling more </t>
   </si>
   <si>
-    <t>A snowstorm approaches. Weather reports have estimated a foot of snow.</t>
-  </si>
-  <si>
     <t>Without much effort, you dip your fingers in your chalice and lightly sprinkle the sparse land below. Your followers scramble out of their dilapidated residence to grab what they can in their dust filled buckets. Fights break out.</t>
   </si>
   <si>
@@ -139,45 +136,18 @@
     <t>You throw a mighty punch to the earth in the quakes opposite direction. Unfortunately, your form was a little shaky and the quake only got stronger.</t>
   </si>
   <si>
-    <t>Quickly strecthing out your hands, you attempt to shake the Earth against the quakes beat but due to your lack of musical talent, you manage to strengthen the quake ten fold!</t>
-  </si>
-  <si>
     <t>Giant robots, who are more than meets the iris, descend from the heavens.</t>
   </si>
   <si>
-    <t>A neighboring nation has initiated an attack against your people. The cause seems to come from their crushing defeat at the last sportsball match.</t>
-  </si>
-  <si>
     <t>A neighboring nation has disrupted your peoples thousand year Yo-Yo trade route.</t>
   </si>
   <si>
-    <t xml:space="preserve">As unimaginative as it may sound, you part the waves of a nearby ocean indefinitly. Unfortunately, you start the wave parting too close to your people's seaport, as a result, essential fishing ships and other vessels topple over. Your people starve… because of your obsession for Yo-Yo's. </t>
-  </si>
-  <si>
-    <t>As unimaginative as it may sound, you part the waves of a nearby ocean indefinitly. Not only does this boom the Yo-Yo trade for your people, it also creates a temporary surplus of food for your people as they simply pluck fish from the oceans walls.</t>
-  </si>
-  <si>
-    <t>To eliminate the problem completely, you decide to rain meteors amongst the neighboring nation. Despite the neighboring nation comitting multiple atrocities, they did not think that they would perish due to a childrens toy. They are eliminated completely and the trade route resumes.</t>
-  </si>
-  <si>
-    <t>To eliminate the problem completely, you decide to rain meteors amongst the neighboring nation. Unbeknowst to you, upper atmosphere winds of approximately 800 miles per hour hurl the meteors off their intended path and end up hitting your followers land. The thousand year old Yo-Yo shop is damaged indefinitly. good job</t>
-  </si>
-  <si>
     <t>Zombie apoc</t>
   </si>
   <si>
     <t>Guy with glowing red stick</t>
   </si>
   <si>
-    <t>You honestly could care less about your people's Yo-Yo trade route as you've recently gotten into Cubing. However, you decide to place a hastily put together vision in the trade masters head in which he slides four inflatable life savers under each leg of a camal in preperation for sea travel as an alternate route. Trade continues again but at a slower pace.</t>
-  </si>
-  <si>
-    <t>You honestly could care less about your people's Yo-Yo trade route as you've recently gotten into Cubing. However, you decide to place a hastily put together vision in the trade masters head in which he slides four inflatable life savers under each leg of a camal in preperation for sea travel as an alternate route. The trade master poorly inteprets the vision (???)</t>
-  </si>
-  <si>
-    <t>You attempt to conjure up a mirage of the Yo-Yo merchants in front of the attackers as a distraction for the attackers. The attackers easily fall for the mirrage, when they finally reach the faux merchants, they are presented with stacks of Yo-Yo catalogues which the attackers never really took the time to look at. They are now interested in opening a trade route with your people.</t>
-  </si>
-  <si>
     <t>You attempt to conjure up a mirage of the Yo-Yo merchants in front of the attackers as a distraction for the attackers. One of the attackers uses their binoculars only to prove that the mirage is nothing but a stack of Yo-Yo catalogues. The attackers are infuriated and now have a personal vendetta against Yo-Yo's and anyone who trades them.</t>
   </si>
   <si>
@@ -320,6 +290,108 @@
   </si>
   <si>
     <t>SHIPWRECK</t>
+  </si>
+  <si>
+    <t>You open a time rift from another dimension and summon the holy tank ready for command by your people.</t>
+  </si>
+  <si>
+    <t>You smite the giant robot with a bolt of lightning, with its batteries recharged it moves on its way for destruction.</t>
+  </si>
+  <si>
+    <t>You summon a drizzle of rain. The robots quickly short circuit and explode.  A few unlucky followers were recipients of shrapnel to their cranial area.</t>
+  </si>
+  <si>
+    <t>As the giant robots descend, you quickly replace the ground below them with quicksand. Your followers fear quickly turns into laughter.</t>
+  </si>
+  <si>
+    <t>Quickly stretching out your hands, you attempt to shake the Earth against the quakes beat but due to your lack of musical talent, you manage to strengthen the quake ten fold!</t>
+  </si>
+  <si>
+    <t>A neighboring nation has initiated an attack against your people. The cause seems to come from their crushing defeat at the last sports ball match.</t>
+  </si>
+  <si>
+    <t>You honestly could care less about your people's Yo-Yo trade route as you've recently gotten into Cubing. However, you decide to place a hastily put together vision in the trade masters head in which he slides four inflatable life savers under each leg of a camel in preparation for sea travel as an alternate route. Trade continues again but at a slower pace.</t>
+  </si>
+  <si>
+    <t>You honestly could care less about your people's Yo-Yo trade route as you've recently gotten into Cubing. However, you decide to place a hastily put together vision in the trade masters head in which he slides four inflatable life savers under each leg of a camel in preparation for sea travel as an alternate route. The trade master poorly interprets the vision (???)</t>
+  </si>
+  <si>
+    <t>You attempt to conjure up a mirage of the Yo-Yo merchants in front of the attackers as a distraction for the attackers. The attackers easily fall for the mirage, when they finally reach the faux merchants, they are presented with stacks of Yo-Yo catalogues which the attackers never really took the time to look at. They are now interested in opening a trade route with your people.</t>
+  </si>
+  <si>
+    <t>As unimaginative as it may sound, you part the waves of a nearby ocean indefinitely. Not only does this boom the Yo-Yo trade for your people, it also creates a temporary surplus of food for your people as they simply pluck fish from the oceans walls.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As unimaginative as it may sound, you part the waves of a nearby ocean indefinitely. Unfortunately, you start the wave parting too close to your people's seaport, as a result, essential fishing ships and other vessels topple over. Your people starve… because of your obsession for Yo-Yo's. </t>
+  </si>
+  <si>
+    <t>To eliminate the problem completely, you decide to rain meteors amongst the neighboring nation. Despite the neighboring nation committing multiple atrocities, they did not think that they would perish due to a children's toy. They are eliminated completely and the trade route resumes.</t>
+  </si>
+  <si>
+    <t>To eliminate the problem completely, you decide to rain meteors amongst the neighboring nation. Unbeknownst to you, upper atmosphere winds of approximately 800 miles per hour hurl the meteors off their intended path and end up hitting your followers land. The thousand year old Yo-Yo shop is damaged indefinitely. good job</t>
+  </si>
+  <si>
+    <t>You send a deadly plague to exterminate the robots, however, the robots are not affected. Your followers become deathly ill.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You perform you roll as the "God of Rock"  by blowing the theoretical roof off. The robots break down in tears according to your magnificent rifts and chords. They leave with intentions of sharing divine tunes with other robot citizens. Your followers are spared. </t>
+  </si>
+  <si>
+    <t>You snap your fingers and the robots spontaneously explode. You quietly yet confidently say "got 'em" as the accompanied wind blows shrapnel into a nearby non-worshiping nation.</t>
+  </si>
+  <si>
+    <t>You snap your fingers and the robots spontaneously explode. You quietly yet confidently say "got 'em… oh wait" as the lack of wind allows shrapnel to rain down on your followers.</t>
+  </si>
+  <si>
+    <t>DRAGON ATTACKS CITY</t>
+  </si>
+  <si>
+    <t>undead mage?</t>
+  </si>
+  <si>
+    <t>Unleash own dragon to fight dragon, many casualties but got to watch a dragon fight</t>
+  </si>
+  <si>
+    <t>One follower claims to be a reincarnation of Your Grace and is speaking in your place.</t>
+  </si>
+  <si>
+    <t>You focus energy from the sun at your peoples land for a few seconds to melt snow. Your followers are relieved that their crops will be spared.</t>
+  </si>
+  <si>
+    <t>An unexpected blizzard hits your peoples land.</t>
+  </si>
+  <si>
+    <t>Out of jealousy for his GORGEOUS hair, you give him bad hair days for the rest of his pitiful existence. A trend is set amongst your followers for this hairstyle.</t>
+  </si>
+  <si>
+    <t>Out of jealousy for his GORGEOUS hair, you give him bad hair days for the rest of his pitiful existence. As a result, his self confidence hinders considerably and he locks himself in his home. Your followers quickly forget about him.</t>
+  </si>
+  <si>
+    <t>You unleash a fire breathing dragon it is untamed but you believe in it.  Due to your negligence, the dragon roasts your followers, however, the snow is clear.</t>
+  </si>
+  <si>
+    <t>You unleash a fire breathing dragon which has been trained for 7 God years.  With precision and accuracy, the dragon breaths fire in specific areas careful to avoid your followers. Your followers are astonished by this act and praise Your Grace.</t>
+  </si>
+  <si>
+    <t>You summon the infamous SAND BIRD which you got as a gift from a merchant who is totally not suspicious which also sold SAND CATS. The Sand Bird quickly swoops in and snatches the Sand Worm. Your followers cannot believe what just happened and place all the (deserved) effort on Your Grace.</t>
+  </si>
+  <si>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>You place firewood on the sun to increase its intensity.  As a result, the snow quickly melts, however, a drought plagues your people. It's the thought that counts.</t>
+  </si>
+  <si>
+    <t>You perform a rite on your followers to prepare them for hibernation as the blizzard approaches. Sometime after the blizzard you nearly forgot about your followers. You quickly use the Sacred Air horn and wake up your followers to enjoy the warm Spring air.</t>
+  </si>
+  <si>
+    <t>You perform a rite on your followers to prepare them for hibernation as the blizzard approaches. However, you forgot to wake them up afterwards and some of your followers starve to death.</t>
+  </si>
+  <si>
+    <t>You send down Holy Shovels of Shoveling which have the ability to quickly cut through snow and (make it feel light as a feather). Knowing that your followers aren't immortal, you attach balloons to each shovel to allow for a safe decent.</t>
+  </si>
+  <si>
+    <t>You send down Holy Shovels of Shoveling which have the ability to quickly cut through snow and (make it feel light as a feather). Unfortunately, the Holy Shovels of Shoveling fall from the heavens at unsafe speeds resulting in impalment.</t>
   </si>
 </sst>
 </file>
@@ -653,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,28 +750,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -710,22 +782,22 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>3</v>
@@ -733,60 +805,60 @@
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -794,28 +866,28 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -823,28 +895,28 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -852,312 +924,312 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="I15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1165,86 +1237,115 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1359,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,52 +1375,52 @@
     </row>
     <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -1335,7 +1436,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,13 +1453,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1369,10 +1470,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1380,13 +1481,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1394,83 +1495,83 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made more entries into the excel sheet
</commit_message>
<xml_diff>
--- a/BadEventsV4ToParse.xlsx
+++ b/BadEventsV4ToParse.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\unitything\Be-a-god\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\banner.main.ad.rit.edu\students\jxs7205\IGMProfile\Desktop\GitHub\Be-a-god\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22575" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22575" windowHeight="7575" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BAD" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="163">
   <si>
     <t>Event</t>
   </si>
@@ -429,7 +429,100 @@
     <t>You made them  disorganized, untrained and hostile to each other. However, it made some of them really dangerous and attack your people</t>
   </si>
   <si>
-    <t>You cut the cheese so bad that it could kill anybody and use your impressive airbending skills to make it stay over the maurading nomads</t>
+    <t>You cut the holy cheese that could kill anybody and use your impressive airbending skills to make it stay over the maurading nomads</t>
+  </si>
+  <si>
+    <t>You cut the holy cheese that could kill anybody and use your impressive airbending skills to make it stay over the maurading nomads, however, a fly broke your concentration and you made it encompass your people too</t>
+  </si>
+  <si>
+    <t>You wanted to confuse the nomads with your confuse ray, however it backfires and they get the great idea of blockading the great yo-yo trade route. Many people have died from a shortage of food…. And yo-yos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You wanted to confuse the nomads with your confuse ray, and it worked. They thought it was a great idea to blockade your greate yo-yo trade route with flowers. In actucally, it brings more people into your cities and of course….. More money. </t>
+  </si>
+  <si>
+    <t>The nomads call upon their God and the both of you have a arm wrestling contest. You lost in the end, and your handprint killed some of your followers and made a new gaping canyon on the very important yo-yo trade route</t>
+  </si>
+  <si>
+    <t>Your attempt to calm down the storm that you caused (What, how can she say that Xbox is better then PS4) came back sucessful, and your even able to some beautiful winds together "wink wink" that helps your followers</t>
+  </si>
+  <si>
+    <t>You clap the air so hard that you are able to cancel out the tornado. Your followers have created a new holiday call "The Lord's Clap Day" in honor of you</t>
+  </si>
+  <si>
+    <t>You clap the air so hard that you make the tornado into a hurricane. Your followers wondered how dumb you could be while they waited for the storm to pass</t>
+  </si>
+  <si>
+    <t>You sprayed a liquid that guarantees to make tornados go away. Instantly you go to buy more as your people praise you for stopping the tornado</t>
+  </si>
+  <si>
+    <t>You sprayed a liquid that guarantees to make tornados go away. Instantly you cringed at the screams and wails of your subjects as you peel away the false label that was on the spray bottle…..</t>
+  </si>
+  <si>
+    <t>Your attempt to calm down the storm that you caused (What, how can she say that Atari 2600 is better then NES) came back unsucessful, in fact, she increased her power.  You hear your people cry as you continue to contemplate whether or not to interfere.....</t>
+  </si>
+  <si>
+    <t>You order the Avatar, the proclaimed "Master of all elements", to help you with your problem. Since he owned you a debt, he "gladly" help you and convince you people that he is your "disciple"…..</t>
+  </si>
+  <si>
+    <t>You order the Avatar, the proclaimed "Master of all elements", to help you with your problem. However, he's still pretty mad at you and increases the speeds of the winds</t>
+  </si>
+  <si>
+    <t>You simply pug up the volcano, and the heat that is coming from the mountain fuel your followers famous "sfefse" springs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You plug up the volcano, unfortunately the plug was made of wood. It easily gives way and the resultant magma spews down on your followers </t>
+  </si>
+  <si>
+    <t>Maybe that huge fire and screams of your people are signs that  dropping that giant rock to try to cover the volcano was not your best idea……</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surprisingly, the volcano is now hidden under the giant rock that you dropped on top of it. Your people sing to you and of your "genius" plan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You send a vision to warn your followers to dig a trench to collect and divert the lava flow. Thanfully, it was received by Nisgith, the highly respected king. And the people were able to divert such a disaster </t>
+  </si>
+  <si>
+    <t>You send a vision to warn your followers to dig a trench to collect and divert the lava flow. It was received by hojors, the town fool. No one paid heed and your followers lose a lot of their important buildings</t>
+  </si>
+  <si>
+    <t>Rolling a 20-sided dice to activiate your godly water powers, you rolled a number that causes a heavy rain to fall on the volcano, thus putting it out forever</t>
+  </si>
+  <si>
+    <t>Rolling a 20-sided dice to activiate your godly water powers, you rolled a 20, the "critical fail", and put your face into your hands as you just expediated the volcano's eruption</t>
+  </si>
+  <si>
+    <t>Staring at a nearby mountain reveals its hidden content to your followers, and they rejoice at the new and improve yo-yos that they now poccess</t>
+  </si>
+  <si>
+    <t>Staring at a nearby mountain reveals its hidden content to your followers, and they gnat their teeth in frustration as a foul odor premeates the air for the next few weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You in your inteligent foresight have told your people to stockpile yo-yos just in case a situation such as this happened. They find it and spread the news of your huge care for the people </t>
+  </si>
+  <si>
+    <t>You in your inteligent foresight have told your people to stockpile yo-yos just in case a situation such as this happened.You just don't remember where it is and your people are mad that you lost some of their most prized possessions.</t>
+  </si>
+  <si>
+    <t>In your frustration in trying to find a solution to this problem, you kick over your chest full of toys. It rains down on your people, and they are at awe at how gracious you are to share.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In your frustration in trying to find a solution to this problem, you kick over your chest full of mousetraps. As the mousetraps fall, your follower look at the horror  at how such an evil contraption could rain down from the heavens </t>
+  </si>
+  <si>
+    <t>Visiting dignitaries</t>
+  </si>
+  <si>
+    <t>Gods visiting from a different Pantheon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love is in the air </t>
+  </si>
+  <si>
+    <t>scientific breakthrough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">movie chronicling your amazing feats </t>
   </si>
 </sst>
 </file>
@@ -577,10 +670,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I21" tableType="xml" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I21" tableType="xml" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" connectionId="1">
   <autoFilter ref="A1:I21"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="badeventsvariation" name="Event" dataDxfId="10">
+    <tableColumn id="1" uniqueName="badeventsvariation" name="Event" dataDxfId="8">
       <xmlColumnPr mapId="1" xpath="/BadeventsCollection/Badevents/Events/@badeventsvariation" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="Response1" name="Outcome 1 Good" dataDxfId="7">
@@ -877,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,62 +1104,62 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>86</v>
+        <v>143</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>86</v>
+        <v>149</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>86</v>
+        <v>146</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1127,7 +1220,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
@@ -1137,44 +1230,46 @@
       <c r="C9" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="E9" s="3" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>131</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>86</v>
+        <v>154</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>86</v>
@@ -1586,10 +1681,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,6 +1822,31 @@
         <v>80</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
testing some of the bad events
</commit_message>
<xml_diff>
--- a/BadEventsV4ToParse.xlsx
+++ b/BadEventsV4ToParse.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22575" windowHeight="7575" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22575" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="BAD" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="181">
   <si>
     <t>Event</t>
   </si>
@@ -483,21 +483,12 @@
     <t xml:space="preserve">You send a vision to warn your followers to dig a trench to collect and divert the lava flow. Thanfully, it was received by Nisgith, the highly respected king. And the people were able to divert such a disaster </t>
   </si>
   <si>
-    <t>You send a vision to warn your followers to dig a trench to collect and divert the lava flow. It was received by hojors, the town fool. No one paid heed and your followers lose a lot of their important buildings</t>
-  </si>
-  <si>
     <t>Rolling a 20-sided dice to activiate your godly water powers, you rolled a number that causes a heavy rain to fall on the volcano, thus putting it out forever</t>
   </si>
   <si>
     <t>Rolling a 20-sided dice to activiate your godly water powers, you rolled a 20, the "critical fail", and put your face into your hands as you just expediated the volcano's eruption</t>
   </si>
   <si>
-    <t>Staring at a nearby mountain reveals its hidden content to your followers, and they rejoice at the new and improve yo-yos that they now poccess</t>
-  </si>
-  <si>
-    <t>Staring at a nearby mountain reveals its hidden content to your followers, and they gnat their teeth in frustration as a foul odor premeates the air for the next few weeks</t>
-  </si>
-  <si>
     <t xml:space="preserve">You in your inteligent foresight have told your people to stockpile yo-yos just in case a situation such as this happened. They find it and spread the news of your huge care for the people </t>
   </si>
   <si>
@@ -523,6 +514,69 @@
   </si>
   <si>
     <t xml:space="preserve">movie chronicling your amazing feats </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listening to the cries of your people, you summoned a giant yo-yo in the middle of town square. It obeys your people, providing joy and happiness for them. It is also an item that the neighborring coutry covets </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listening to the cries of your people, you summoned a giant yo-yo in the middle of town square.However, It starts to rampage and destorys some of your people and their buildings. </t>
+  </si>
+  <si>
+    <t>Staring at a nearby mountain reveals its hidden content to your followers. They rejoice at the new and improve yo-yos that they now poccess</t>
+  </si>
+  <si>
+    <t>Staring at a nearby mountain reveals its hidden content to your followers. They gnat their teeth in frustration as a foul odor premeates the air for the next few weeks</t>
+  </si>
+  <si>
+    <t>When he claims to be better then you in League of Legends, that is when you draw the line. You challenge him to a 1v1 and impress your people with your impressive skills</t>
+  </si>
+  <si>
+    <t>When he claims to be better then you in League of Legends, that is when you draw the line. You challenge him to a 1v1 and embarras yourself when he starts dancing over your champion's dead body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Imposter seems to start flirting with one of the lady followers that you had your eyes on.  You instantly show your machismo and win the lady, and as you give her a night she won't forget, she starts spreading the news of your amazing skills </t>
+  </si>
+  <si>
+    <t>You send a vision to warn your followers to dig a trench to collect and divert the lava flow. It was received by Hojors, the town fool. No one paid heed and your followers lose a lot of their important buildings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Imposter seems to start flirting with one of the lady followers that you had your eyes on.  You try to show your machismo and win the lady, but you embarras yourself and she spreads the news of the laughable exchange you two had </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You simply get fed up with what he is doing and challenge him to the ultimate battle of DDR. You (rigged) showed off your skills to the people who are at awe, and finally put the imposter in his place </t>
+  </si>
+  <si>
+    <t>You simply get fed up with what he is doing and challenge him to the ultimate battle of DDR. You rigged the machine to make you win, but as taunt him showing your moves to the imposter, the machine explodes in your face and destorys some buildings</t>
+  </si>
+  <si>
+    <t>They seem to be docile enough. So you instruct your followers to herd them to the fields, where they continue to gaze and provide food for your people</t>
+  </si>
+  <si>
+    <t>They seem to be docile enough. So you instruct your followers to herd them to the fields. Unfortunately, they turn out to be disguised thieves  and steal some of your town's prized possessions and statues of you in the middle of the night</t>
+  </si>
+  <si>
+    <t>At the sight of the sheeps you grow hungry, so you ordered your followers to hastily  sacrifice one of them to you. As they start the ritual, the sheep's defense mechanisms kick in, transforminging him into a gaint man-killing sheep who terrorize your people</t>
+  </si>
+  <si>
+    <t>At the sight of the sheeps you grow hungry, so you ordered your followers to hastily  sacrifice one of them to you. As they start the ritual, the sheep's defense mechanisms kick in but messes up, transforminging him into a gaint sheep which you share with the people</t>
+  </si>
+  <si>
+    <t>As your town goes to slaughter the sheep for food, it is reveled that one of the sheep is the personal pet of udpof, the God of the wopesde people. Using your impressive charisma, you negoiate a way for your followers to feast on the delicious sheep while returning the pet</t>
+  </si>
+  <si>
+    <t>As your town goes to slaughter the sheep for food, it is reveled that one of the sheep is the personal pet of udpof, the God of the wopesde people. During your negoiations, you sneezed in his face, which is an insult in his eyes. With him saying the magic words, his pet starts destroying your people</t>
+  </si>
+  <si>
+    <t>You instruct your people to save some of the sheep for their wool. While they go to shear them, they get infected by a virus that transmit through the touch of their wool. The people cry on how you let this happen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You instruct your people to save some of the sheep for their wool. While they go to shear them, they see that one of sheep's wool was used to hide treasure, lots of it. Your followers are happy from this terricfic outcome </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking directly at the fire, you start sheding tears that rains down and put out the fire. Your followers thank you for your grace </t>
+  </si>
+  <si>
+    <t>Looking directly at the fire, you start sheding tears that rains down and put out the fire, but you continue and flood some parts of your land</t>
   </si>
 </sst>
 </file>
@@ -970,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1201,7 @@
         <v>148</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>147</v>
@@ -1156,10 +1210,10 @@
         <v>146</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1191,7 +1245,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>108</v>
       </c>
@@ -1202,22 +1256,22 @@
         <v>112</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>86</v>
+        <v>166</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1254,28 +1308,28 @@
         <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="H10" s="3" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>86</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1419,44 +1473,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>86</v>
+        <v>180</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>86</v>
@@ -1683,7 +1737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1824,27 +1878,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
good events, not on screen yet
</commit_message>
<xml_diff>
--- a/BadEventsV4ToParse.xlsx
+++ b/BadEventsV4ToParse.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22575" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22575" windowHeight="7575" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BAD" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="173">
   <si>
     <t>Event</t>
   </si>
@@ -468,9 +468,6 @@
     <t>You order the Avatar, the proclaimed "Master of all elements", to help you with your problem. However, he's still pretty mad at you and increases the speeds of the winds</t>
   </si>
   <si>
-    <t>You simply pug up the volcano, and the heat that is coming from the mountain fuel your followers famous "sfefse" springs</t>
-  </si>
-  <si>
     <t xml:space="preserve">You plug up the volcano, unfortunately the plug was made of wood. It easily gives way and the resultant magma spews down on your followers </t>
   </si>
   <si>
@@ -489,18 +486,6 @@
     <t>Rolling a 20-sided dice to activiate your godly water powers, you rolled a 20, the "critical fail", and put your face into your hands as you just expediated the volcano's eruption</t>
   </si>
   <si>
-    <t xml:space="preserve">You in your inteligent foresight have told your people to stockpile yo-yos just in case a situation such as this happened. They find it and spread the news of your huge care for the people </t>
-  </si>
-  <si>
-    <t>You in your inteligent foresight have told your people to stockpile yo-yos just in case a situation such as this happened.You just don't remember where it is and your people are mad that you lost some of their most prized possessions.</t>
-  </si>
-  <si>
-    <t>In your frustration in trying to find a solution to this problem, you kick over your chest full of toys. It rains down on your people, and they are at awe at how gracious you are to share.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In your frustration in trying to find a solution to this problem, you kick over your chest full of mousetraps. As the mousetraps fall, your follower look at the horror  at how such an evil contraption could rain down from the heavens </t>
-  </si>
-  <si>
     <t>Visiting dignitaries</t>
   </si>
   <si>
@@ -516,18 +501,6 @@
     <t xml:space="preserve">movie chronicling your amazing feats </t>
   </si>
   <si>
-    <t xml:space="preserve">Listening to the cries of your people, you summoned a giant yo-yo in the middle of town square. It obeys your people, providing joy and happiness for them. It is also an item that the neighborring coutry covets </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listening to the cries of your people, you summoned a giant yo-yo in the middle of town square.However, It starts to rampage and destorys some of your people and their buildings. </t>
-  </si>
-  <si>
-    <t>Staring at a nearby mountain reveals its hidden content to your followers. They rejoice at the new and improve yo-yos that they now poccess</t>
-  </si>
-  <si>
-    <t>Staring at a nearby mountain reveals its hidden content to your followers. They gnat their teeth in frustration as a foul odor premeates the air for the next few weeks</t>
-  </si>
-  <si>
     <t>When he claims to be better then you in League of Legends, that is when you draw the line. You challenge him to a 1v1 and impress your people with your impressive skills</t>
   </si>
   <si>
@@ -577,6 +550,9 @@
   </si>
   <si>
     <t>Looking directly at the fire, you start sheding tears that rains down and put out the fire, but you continue and flood some parts of your land</t>
+  </si>
+  <si>
+    <t>You simply plug up the volcano, and the heat that is coming from the mountain fuel your followers famous "sfefse" springs</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I21"/>
+    <sheetView topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,28 +1168,28 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1256,22 +1232,22 @@
         <v>112</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1303,63 +1279,47 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>162</v>
+        <v>94</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>163</v>
+        <v>95</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>151</v>
+        <v>96</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>152</v>
+        <v>40</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>153</v>
+        <v>97</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>160</v>
+        <v>99</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1478,28 +1438,28 @@
         <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1507,10 +1467,10 @@
         <v>49</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>86</v>
@@ -1737,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,27 +1838,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
making the deifferent events text show up
</commit_message>
<xml_diff>
--- a/BadEventsV4ToParse.xlsx
+++ b/BadEventsV4ToParse.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22575" windowHeight="7575" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22575" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="BAD" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="175">
   <si>
     <t>Event</t>
   </si>
@@ -553,6 +553,12 @@
   </si>
   <si>
     <t>You simply plug up the volcano, and the heat that is coming from the mountain fuel your followers famous "sfefse" springs</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You saw him trying to command your followers in giving him things. </t>
   </si>
 </sst>
 </file>
@@ -1000,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,13 +1319,27 @@
         <v>93</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1384,7 +1404,7 @@
         <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>86</v>
@@ -1421,14 +1441,18 @@
       <c r="D15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="F15" s="3" t="s">
         <v>86</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="I15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1697,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>